<commit_message>
Changes for positive difference
</commit_message>
<xml_diff>
--- a/NewFile.xlsx
+++ b/NewFile.xlsx
@@ -169,7 +169,7 @@
         <v>189.0</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>-9.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="3">
@@ -192,7 +192,7 @@
         <v>171.0</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>-11.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>